<commit_message>
Updated testing for type 1
</commit_message>
<xml_diff>
--- a/transactions_upload.xlsx
+++ b/transactions_upload.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidal-gurnawi/Documents/data_science/agentic_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidal-gurnawi/Documents/data_science/agentic_workflows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39948C85-2EE9-A54D-B6C1-56869185D2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6D2B13-9FFD-1041-B96C-2D786A231424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="620" windowWidth="34400" windowHeight="28180" activeTab="1" xr2:uid="{A52D9AD8-0393-0A4D-90C8-B93F7153FAEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts receivable ledger" sheetId="3" r:id="rId1"/>
-    <sheet name="Customers" sheetId="4" r:id="rId2"/>
-    <sheet name="Payments" sheetId="6" r:id="rId3"/>
+    <sheet name="Test results" sheetId="7" r:id="rId2"/>
+    <sheet name="Customers" sheetId="4" r:id="rId3"/>
+    <sheet name="Payments" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>05.01.2025</t>
   </si>
@@ -251,6 +251,57 @@
   </si>
   <si>
     <t>discount_amount</t>
+  </si>
+  <si>
+    <t>Workflow type</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>228m</t>
+  </si>
+  <si>
+    <t>Type 5</t>
+  </si>
+  <si>
+    <t>227m</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Qwen3:8b</t>
+  </si>
+  <si>
+    <t>Type 1</t>
+  </si>
+  <si>
+    <t>llama3.1:8bn</t>
+  </si>
+  <si>
+    <t>5m</t>
+  </si>
+  <si>
+    <t>qwen3:8bn</t>
+  </si>
+  <si>
+    <t>83m</t>
+  </si>
+  <si>
+    <t>deepseek-r1:14b</t>
+  </si>
+  <si>
+    <t>32m</t>
+  </si>
+  <si>
+    <t>gpt-oss:20b</t>
   </si>
 </sst>
 </file>
@@ -286,8 +337,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,7 +678,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,10 +1003,130 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9E767A-B394-0C48-847D-5A71C5B0C521}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2CB4A3-F908-1741-AEA9-BDFE2AAFF611}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1153,12 +1326,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CD3250-FDFA-A24D-BDC8-A2E78F64D479}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated testing for type 5
</commit_message>
<xml_diff>
--- a/transactions_upload.xlsx
+++ b/transactions_upload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidal-gurnawi/Documents/data_science/agentic_workflows/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6D2B13-9FFD-1041-B96C-2D786A231424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83413A01-3433-3A45-B340-8E5EC56AB00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="620" windowWidth="34400" windowHeight="28180" activeTab="1" xr2:uid="{A52D9AD8-0393-0A4D-90C8-B93F7153FAEC}"/>
+    <workbookView xWindow="34400" yWindow="600" windowWidth="34400" windowHeight="26560" activeTab="1" xr2:uid="{A52D9AD8-0393-0A4D-90C8-B93F7153FAEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts receivable ledger" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Customers" sheetId="4" r:id="rId3"/>
     <sheet name="Payments" sheetId="6" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test results'!$A$1:$E$17</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="99">
   <si>
     <t>05.01.2025</t>
   </si>
@@ -265,15 +268,6 @@
     <t>Instance</t>
   </si>
   <si>
-    <t>228m</t>
-  </si>
-  <si>
-    <t>Type 5</t>
-  </si>
-  <si>
-    <t>227m</t>
-  </si>
-  <si>
     <t>Accuracy</t>
   </si>
   <si>
@@ -302,6 +296,48 @@
   </si>
   <si>
     <t>gpt-oss:20b</t>
+  </si>
+  <si>
+    <t>220m</t>
+  </si>
+  <si>
+    <t>192m</t>
+  </si>
+  <si>
+    <t>525m</t>
+  </si>
+  <si>
+    <t>183m</t>
+  </si>
+  <si>
+    <t>Type 4</t>
+  </si>
+  <si>
+    <t>Type 3</t>
+  </si>
+  <si>
+    <t>Type 2</t>
+  </si>
+  <si>
+    <t>2m</t>
+  </si>
+  <si>
+    <t>11m</t>
+  </si>
+  <si>
+    <t>50m</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <t>9m</t>
+  </si>
+  <si>
+    <t>45m</t>
   </si>
 </sst>
 </file>
@@ -337,10 +373,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,15 +1042,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9E767A-B394-0C48-847D-5A71C5B0C521}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="20.5" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1030,60 +1069,72 @@
         <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="3">
+        <v>46327</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>87</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1">
-        <v>46027</v>
+        <v>46034</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1">
-        <v>46027</v>
+        <v>46033</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1">
-        <v>46027</v>
+        <v>46033</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -1091,16 +1142,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="1">
-        <v>46027</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
@@ -1108,16 +1157,179 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" t="s">
         <v>80</v>
       </c>
-      <c r="B7" s="1">
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="1">
         <v>46027</v>
       </c>
-      <c r="C7" t="s">
-        <v>87</v>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1">
+        <v>46027</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E17" xr:uid="{8A9E767A-B394-0C48-847D-5A71C5B0C521}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1328,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1CD3250-FDFA-A24D-BDC8-A2E78F64D479}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1342,7 +1554,7 @@
     <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1356,7 +1568,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>948347</v>
       </c>
@@ -1369,8 +1581,11 @@
       <c r="D2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>34847</v>
       </c>
@@ -1383,8 +1598,11 @@
       <c r="D3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>29304</v>
       </c>
@@ -1397,8 +1615,11 @@
       <c r="D4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3837459</v>
       </c>
@@ -1411,8 +1632,11 @@
       <c r="D5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>390576</v>
       </c>
@@ -1425,8 +1649,11 @@
       <c r="D6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>302947</v>
       </c>
@@ -1439,8 +1666,11 @@
       <c r="D7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>39506</v>
       </c>
@@ -1453,8 +1683,11 @@
       <c r="D8" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2394759</v>
       </c>
@@ -1468,7 +1701,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>390475</v>
       </c>
@@ -1480,6 +1713,14 @@
       </c>
       <c r="D10" t="s">
         <v>53</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" s="4">
+        <v>46243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>